<commit_message>
Added shadow to box. Updated map so it would contain all box platform.
</commit_message>
<xml_diff>
--- a/Do-an-cuoi-ky_SE102/Map/Map1-1.xlsx
+++ b/Do-an-cuoi-ky_SE102/Map/Map1-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phong\source\repos\gamedev-intro-tutorials\05-SceneManager\Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phong\source\repos\Do-an-cuoi-ky_SE102\Do-an-cuoi-ky_SE102\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFE4C1F7-64A6-4D22-9F4F-8530A007AF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270A8D17-D880-48C9-A93E-39F0738C0080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{18652980-8A0A-46A1-B3A6-355C8E1B5B9D}"/>
+    <workbookView xWindow="1665" yWindow="4845" windowWidth="17280" windowHeight="10073" xr2:uid="{18652980-8A0A-46A1-B3A6-355C8E1B5B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOX </t>
+  </si>
+  <si>
+    <t>PLATFORM</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,8 +59,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -60,6 +78,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -76,9 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F42E79-6207-450F-8948-543BB6439B66}">
-  <dimension ref="A1:AH39"/>
+  <dimension ref="A1:BC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="AQ13" sqref="AQ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -426,9 +452,11 @@
     <col min="20" max="20" width="9.06640625" style="1"/>
     <col min="25" max="25" width="9.06640625" style="1"/>
     <col min="30" max="30" width="9.06640625" style="1"/>
+    <col min="35" max="35" width="9.06640625" style="3"/>
+    <col min="36" max="36" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>1</v>
       </c>
@@ -436,11 +464,14 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D1">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="F1">
         <v>1</v>
       </c>
@@ -448,7 +479,7 @@
         <v>624</v>
       </c>
       <c r="H1">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I1">
         <v>0</v>
@@ -460,7 +491,7 @@
         <v>624</v>
       </c>
       <c r="M1">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N1">
         <v>3</v>
@@ -472,7 +503,7 @@
         <v>1152</v>
       </c>
       <c r="R1">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S1">
         <v>3</v>
@@ -484,7 +515,7 @@
         <v>1536</v>
       </c>
       <c r="W1">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="X1">
         <v>3</v>
@@ -496,7 +527,7 @@
         <v>1664</v>
       </c>
       <c r="AB1">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC1">
         <v>3</v>
@@ -508,13 +539,73 @@
         <v>2256</v>
       </c>
       <c r="AG1">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AJ1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK1">
+        <v>6</v>
+      </c>
+      <c r="AL1">
+        <v>272</v>
+      </c>
+      <c r="AM1">
+        <v>336</v>
+      </c>
+      <c r="AN1">
+        <v>16</v>
+      </c>
+      <c r="AO1">
+        <v>16</v>
+      </c>
+      <c r="AP1">
+        <v>3</v>
+      </c>
+      <c r="AQ1">
+        <v>5</v>
+      </c>
+      <c r="AR1">
+        <v>61002</v>
+      </c>
+      <c r="AS1">
+        <v>62002</v>
+      </c>
+      <c r="AT1">
+        <v>63002</v>
+      </c>
+      <c r="AU1">
+        <v>64002</v>
+      </c>
+      <c r="AV1">
+        <v>65002</v>
+      </c>
+      <c r="AW1">
+        <v>66002</v>
+      </c>
+      <c r="AX1">
+        <v>67002</v>
+      </c>
+      <c r="AY1">
+        <v>68002</v>
+      </c>
+      <c r="AZ1">
+        <v>69002</v>
+      </c>
+      <c r="BA1">
+        <v>60051</v>
+      </c>
+      <c r="BB1">
+        <v>60052</v>
+      </c>
+      <c r="BC1">
+        <v>60052</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -522,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -534,7 +625,7 @@
         <v>640</v>
       </c>
       <c r="H2">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -546,7 +637,7 @@
         <v>640</v>
       </c>
       <c r="M2">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N2">
         <v>4</v>
@@ -558,7 +649,7 @@
         <v>1168</v>
       </c>
       <c r="R2">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S2">
         <v>4</v>
@@ -570,7 +661,7 @@
         <v>1552</v>
       </c>
       <c r="W2">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="X2">
         <v>4</v>
@@ -582,7 +673,7 @@
         <v>1680</v>
       </c>
       <c r="AB2">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC2">
         <v>4</v>
@@ -594,13 +685,73 @@
         <v>2272</v>
       </c>
       <c r="AG2">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AJ2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK2">
+        <v>6</v>
+      </c>
+      <c r="AL2">
+        <v>240</v>
+      </c>
+      <c r="AM2">
+        <v>368</v>
+      </c>
+      <c r="AN2">
+        <v>16</v>
+      </c>
+      <c r="AO2">
+        <v>16</v>
+      </c>
+      <c r="AP2">
+        <v>3</v>
+      </c>
+      <c r="AQ2">
+        <v>3</v>
+      </c>
+      <c r="AR2">
+        <v>61000</v>
+      </c>
+      <c r="AS2">
+        <v>62000</v>
+      </c>
+      <c r="AT2">
+        <v>63000</v>
+      </c>
+      <c r="AU2">
+        <v>64000</v>
+      </c>
+      <c r="AV2">
+        <v>65000</v>
+      </c>
+      <c r="AW2">
+        <v>66000</v>
+      </c>
+      <c r="AX2">
+        <v>67000</v>
+      </c>
+      <c r="AY2">
+        <v>68000</v>
+      </c>
+      <c r="AZ2">
+        <v>69000</v>
+      </c>
+      <c r="BA2">
+        <v>60021</v>
+      </c>
+      <c r="BB2">
+        <v>60022</v>
+      </c>
+      <c r="BC2">
+        <v>60023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -608,7 +759,7 @@
         <v>32</v>
       </c>
       <c r="C3">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -620,7 +771,7 @@
         <v>656</v>
       </c>
       <c r="H3">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -632,7 +783,7 @@
         <v>656</v>
       </c>
       <c r="M3">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N3">
         <v>4</v>
@@ -644,7 +795,7 @@
         <v>1184</v>
       </c>
       <c r="R3">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S3">
         <v>4</v>
@@ -656,7 +807,7 @@
         <v>1568</v>
       </c>
       <c r="W3">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="X3">
         <v>4</v>
@@ -668,7 +819,7 @@
         <v>1696</v>
       </c>
       <c r="AB3">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC3">
         <v>4</v>
@@ -680,13 +831,13 @@
         <v>2288</v>
       </c>
       <c r="AG3">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -694,7 +845,7 @@
         <v>48</v>
       </c>
       <c r="C4">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -706,7 +857,7 @@
         <v>672</v>
       </c>
       <c r="H4">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -718,7 +869,7 @@
         <v>672</v>
       </c>
       <c r="M4">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N4">
         <v>4</v>
@@ -730,7 +881,7 @@
         <v>1200</v>
       </c>
       <c r="R4">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S4">
         <v>4</v>
@@ -742,7 +893,7 @@
         <v>1584</v>
       </c>
       <c r="W4">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="X4">
         <v>4</v>
@@ -754,7 +905,7 @@
         <v>1712</v>
       </c>
       <c r="AB4">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC4">
         <v>4</v>
@@ -766,13 +917,70 @@
         <v>2304</v>
       </c>
       <c r="AG4">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK4">
+        <v>6</v>
+      </c>
+      <c r="AL4">
+        <v>1328</v>
+      </c>
+      <c r="AM4">
+        <v>320</v>
+      </c>
+      <c r="AN4">
+        <v>16</v>
+      </c>
+      <c r="AO4">
+        <v>16</v>
+      </c>
+      <c r="AP4">
+        <v>7</v>
+      </c>
+      <c r="AQ4">
+        <v>6</v>
+      </c>
+      <c r="AR4">
+        <v>61002</v>
+      </c>
+      <c r="AS4">
+        <v>62002</v>
+      </c>
+      <c r="AT4">
+        <v>63002</v>
+      </c>
+      <c r="AU4">
+        <v>64002</v>
+      </c>
+      <c r="AV4">
+        <v>65002</v>
+      </c>
+      <c r="AW4">
+        <v>66002</v>
+      </c>
+      <c r="AX4">
+        <v>67002</v>
+      </c>
+      <c r="AY4">
+        <v>68002</v>
+      </c>
+      <c r="AZ4">
+        <v>69002</v>
+      </c>
+      <c r="BA4">
+        <v>60051</v>
+      </c>
+      <c r="BB4">
+        <v>60052</v>
+      </c>
+      <c r="BC4">
+        <v>60052</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -780,7 +988,7 @@
         <v>64</v>
       </c>
       <c r="C5">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -792,7 +1000,7 @@
         <v>688</v>
       </c>
       <c r="H5">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -804,7 +1012,7 @@
         <v>688</v>
       </c>
       <c r="M5">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N5">
         <v>4</v>
@@ -816,7 +1024,7 @@
         <v>1216</v>
       </c>
       <c r="R5">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S5">
         <v>4</v>
@@ -828,7 +1036,7 @@
         <v>1600</v>
       </c>
       <c r="W5">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="X5">
         <v>5</v>
@@ -840,7 +1048,7 @@
         <v>1728</v>
       </c>
       <c r="AB5">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC5">
         <v>4</v>
@@ -852,13 +1060,70 @@
         <v>2320</v>
       </c>
       <c r="AG5">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK5">
+        <v>6</v>
+      </c>
+      <c r="AL5">
+        <v>1296</v>
+      </c>
+      <c r="AM5">
+        <v>352</v>
+      </c>
+      <c r="AN5">
+        <v>16</v>
+      </c>
+      <c r="AO5">
+        <v>16</v>
+      </c>
+      <c r="AP5">
+        <v>7</v>
+      </c>
+      <c r="AQ5">
+        <v>4</v>
+      </c>
+      <c r="AR5">
+        <v>61000</v>
+      </c>
+      <c r="AS5">
+        <v>62000</v>
+      </c>
+      <c r="AT5">
+        <v>63000</v>
+      </c>
+      <c r="AU5">
+        <v>64000</v>
+      </c>
+      <c r="AV5">
+        <v>65000</v>
+      </c>
+      <c r="AW5">
+        <v>66000</v>
+      </c>
+      <c r="AX5">
+        <v>67000</v>
+      </c>
+      <c r="AY5">
+        <v>68000</v>
+      </c>
+      <c r="AZ5">
+        <v>69000</v>
+      </c>
+      <c r="BA5">
+        <v>60021</v>
+      </c>
+      <c r="BB5">
+        <v>60022</v>
+      </c>
+      <c r="BC5">
+        <v>60023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -866,7 +1131,7 @@
         <v>80</v>
       </c>
       <c r="C6">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -878,7 +1143,7 @@
         <v>704</v>
       </c>
       <c r="H6">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -890,7 +1155,7 @@
         <v>704</v>
       </c>
       <c r="M6">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N6">
         <v>4</v>
@@ -902,7 +1167,7 @@
         <v>1232</v>
       </c>
       <c r="R6">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S6">
         <v>4</v>
@@ -914,7 +1179,7 @@
         <v>1744</v>
       </c>
       <c r="AB6">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC6">
         <v>4</v>
@@ -926,13 +1191,70 @@
         <v>2336</v>
       </c>
       <c r="AG6">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK6">
+        <v>6</v>
+      </c>
+      <c r="AL6">
+        <v>1264</v>
+      </c>
+      <c r="AM6">
+        <v>384</v>
+      </c>
+      <c r="AN6">
+        <v>16</v>
+      </c>
+      <c r="AO6">
+        <v>16</v>
+      </c>
+      <c r="AP6">
+        <v>7</v>
+      </c>
+      <c r="AQ6">
+        <v>2</v>
+      </c>
+      <c r="AR6">
+        <v>61001</v>
+      </c>
+      <c r="AS6">
+        <v>62001</v>
+      </c>
+      <c r="AT6">
+        <v>63001</v>
+      </c>
+      <c r="AU6">
+        <v>64001</v>
+      </c>
+      <c r="AV6">
+        <v>65001</v>
+      </c>
+      <c r="AW6">
+        <v>66001</v>
+      </c>
+      <c r="AX6">
+        <v>67001</v>
+      </c>
+      <c r="AY6">
+        <v>68001</v>
+      </c>
+      <c r="AZ6">
+        <v>69001</v>
+      </c>
+      <c r="BA6">
+        <v>60001</v>
+      </c>
+      <c r="BB6">
+        <v>60002</v>
+      </c>
+      <c r="BC6">
+        <v>60003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -940,7 +1262,7 @@
         <v>96</v>
       </c>
       <c r="C7">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -952,7 +1274,7 @@
         <v>720</v>
       </c>
       <c r="H7">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -964,7 +1286,7 @@
         <v>720</v>
       </c>
       <c r="M7">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N7">
         <v>4</v>
@@ -976,7 +1298,7 @@
         <v>1248</v>
       </c>
       <c r="R7">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S7">
         <v>4</v>
@@ -988,7 +1310,7 @@
         <v>1760</v>
       </c>
       <c r="AB7">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC7">
         <v>4</v>
@@ -1000,13 +1322,13 @@
         <v>2352</v>
       </c>
       <c r="AG7">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1014,7 +1336,7 @@
         <v>112</v>
       </c>
       <c r="C8">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -1026,7 +1348,7 @@
         <v>736</v>
       </c>
       <c r="H8">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1038,7 +1360,7 @@
         <v>736</v>
       </c>
       <c r="M8">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N8">
         <v>4</v>
@@ -1050,7 +1372,7 @@
         <v>1264</v>
       </c>
       <c r="R8">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S8">
         <v>4</v>
@@ -1062,7 +1384,7 @@
         <v>1776</v>
       </c>
       <c r="AB8">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC8">
         <v>4</v>
@@ -1074,13 +1396,70 @@
         <v>2368</v>
       </c>
       <c r="AG8">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK8">
+        <v>6</v>
+      </c>
+      <c r="AL8">
+        <v>512</v>
+      </c>
+      <c r="AM8">
+        <v>304</v>
+      </c>
+      <c r="AN8">
+        <v>16</v>
+      </c>
+      <c r="AO8">
+        <v>16</v>
+      </c>
+      <c r="AP8">
+        <v>4</v>
+      </c>
+      <c r="AQ8">
+        <v>7</v>
+      </c>
+      <c r="AR8">
+        <v>61003</v>
+      </c>
+      <c r="AS8">
+        <v>62003</v>
+      </c>
+      <c r="AT8">
+        <v>63003</v>
+      </c>
+      <c r="AU8">
+        <v>64003</v>
+      </c>
+      <c r="AV8">
+        <v>65003</v>
+      </c>
+      <c r="AW8">
+        <v>66003</v>
+      </c>
+      <c r="AX8">
+        <v>67003</v>
+      </c>
+      <c r="AY8">
+        <v>68003</v>
+      </c>
+      <c r="AZ8">
+        <v>69003</v>
+      </c>
+      <c r="BA8">
+        <v>60051</v>
+      </c>
+      <c r="BB8">
+        <v>60052</v>
+      </c>
+      <c r="BC8">
+        <v>60052</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1088,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="C9">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1100,7 +1479,7 @@
         <v>752</v>
       </c>
       <c r="H9">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1112,7 +1491,7 @@
         <v>752</v>
       </c>
       <c r="M9">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N9">
         <v>4</v>
@@ -1124,7 +1503,7 @@
         <v>1280</v>
       </c>
       <c r="R9">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S9">
         <v>4</v>
@@ -1136,7 +1515,7 @@
         <v>1792</v>
       </c>
       <c r="AB9">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC9">
         <v>4</v>
@@ -1148,13 +1527,70 @@
         <v>2384</v>
       </c>
       <c r="AG9">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK9">
+        <v>6</v>
+      </c>
+      <c r="AL9">
+        <v>464</v>
+      </c>
+      <c r="AM9">
+        <v>336</v>
+      </c>
+      <c r="AN9">
+        <v>16</v>
+      </c>
+      <c r="AO9">
+        <v>16</v>
+      </c>
+      <c r="AP9">
+        <v>4</v>
+      </c>
+      <c r="AQ9">
+        <v>5</v>
+      </c>
+      <c r="AR9">
+        <v>61000</v>
+      </c>
+      <c r="AS9">
+        <v>62000</v>
+      </c>
+      <c r="AT9">
+        <v>63000</v>
+      </c>
+      <c r="AU9">
+        <v>64000</v>
+      </c>
+      <c r="AV9">
+        <v>65000</v>
+      </c>
+      <c r="AW9">
+        <v>66000</v>
+      </c>
+      <c r="AX9">
+        <v>67000</v>
+      </c>
+      <c r="AY9">
+        <v>68000</v>
+      </c>
+      <c r="AZ9">
+        <v>69000</v>
+      </c>
+      <c r="BA9">
+        <v>60031</v>
+      </c>
+      <c r="BB9">
+        <v>60032</v>
+      </c>
+      <c r="BC9">
+        <v>60033</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1162,7 +1598,7 @@
         <v>144</v>
       </c>
       <c r="C10">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -1174,7 +1610,7 @@
         <v>768</v>
       </c>
       <c r="H10">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1186,7 +1622,7 @@
         <v>768</v>
       </c>
       <c r="M10">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N10">
         <v>4</v>
@@ -1198,7 +1634,7 @@
         <v>1296</v>
       </c>
       <c r="R10">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S10">
         <v>4</v>
@@ -1210,7 +1646,7 @@
         <v>1808</v>
       </c>
       <c r="AB10">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC10">
         <v>4</v>
@@ -1222,13 +1658,70 @@
         <v>2400</v>
       </c>
       <c r="AG10">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK10">
+        <v>6</v>
+      </c>
+      <c r="AL10">
+        <v>400</v>
+      </c>
+      <c r="AM10">
+        <v>368</v>
+      </c>
+      <c r="AN10">
+        <v>16</v>
+      </c>
+      <c r="AO10">
+        <v>16</v>
+      </c>
+      <c r="AP10">
+        <v>5</v>
+      </c>
+      <c r="AQ10">
+        <v>3</v>
+      </c>
+      <c r="AR10">
+        <v>61001</v>
+      </c>
+      <c r="AS10">
+        <v>62001</v>
+      </c>
+      <c r="AT10">
+        <v>63001</v>
+      </c>
+      <c r="AU10">
+        <v>64001</v>
+      </c>
+      <c r="AV10">
+        <v>65001</v>
+      </c>
+      <c r="AW10">
+        <v>66001</v>
+      </c>
+      <c r="AX10">
+        <v>67001</v>
+      </c>
+      <c r="AY10">
+        <v>68001</v>
+      </c>
+      <c r="AZ10">
+        <v>69001</v>
+      </c>
+      <c r="BA10">
+        <v>60001</v>
+      </c>
+      <c r="BB10">
+        <v>60002</v>
+      </c>
+      <c r="BC10">
+        <v>60003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1236,7 +1729,7 @@
         <v>160</v>
       </c>
       <c r="C11">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -1248,7 +1741,7 @@
         <v>784</v>
       </c>
       <c r="H11">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1260,7 +1753,7 @@
         <v>784</v>
       </c>
       <c r="M11">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N11">
         <v>4</v>
@@ -1272,7 +1765,7 @@
         <v>1312</v>
       </c>
       <c r="R11">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S11">
         <v>4</v>
@@ -1284,7 +1777,7 @@
         <v>1824</v>
       </c>
       <c r="AB11">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC11">
         <v>4</v>
@@ -1296,13 +1789,70 @@
         <v>2416</v>
       </c>
       <c r="AG11">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK11">
+        <v>6</v>
+      </c>
+      <c r="AL11">
+        <v>512</v>
+      </c>
+      <c r="AM11">
+        <v>384</v>
+      </c>
+      <c r="AN11">
+        <v>16</v>
+      </c>
+      <c r="AO11">
+        <v>16</v>
+      </c>
+      <c r="AP11">
+        <v>6</v>
+      </c>
+      <c r="AQ11">
+        <v>2</v>
+      </c>
+      <c r="AR11">
+        <v>61001</v>
+      </c>
+      <c r="AS11">
+        <v>62001</v>
+      </c>
+      <c r="AT11">
+        <v>63001</v>
+      </c>
+      <c r="AU11">
+        <v>64001</v>
+      </c>
+      <c r="AV11">
+        <v>65001</v>
+      </c>
+      <c r="AW11">
+        <v>66001</v>
+      </c>
+      <c r="AX11">
+        <v>67001</v>
+      </c>
+      <c r="AY11">
+        <v>68001</v>
+      </c>
+      <c r="AZ11">
+        <v>69001</v>
+      </c>
+      <c r="BA11">
+        <v>60051</v>
+      </c>
+      <c r="BB11">
+        <v>60052</v>
+      </c>
+      <c r="BC11">
+        <v>60052</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1310,7 +1860,7 @@
         <v>176</v>
       </c>
       <c r="C12">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -1322,7 +1872,7 @@
         <v>800</v>
       </c>
       <c r="H12">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1334,7 +1884,7 @@
         <v>800</v>
       </c>
       <c r="M12">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N12">
         <v>4</v>
@@ -1346,7 +1896,7 @@
         <v>1328</v>
       </c>
       <c r="R12">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S12">
         <v>4</v>
@@ -1358,7 +1908,7 @@
         <v>1840</v>
       </c>
       <c r="AB12">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC12">
         <v>4</v>
@@ -1370,13 +1920,13 @@
         <v>2432</v>
       </c>
       <c r="AG12">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1384,7 +1934,7 @@
         <v>192</v>
       </c>
       <c r="C13">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -1396,7 +1946,7 @@
         <v>816</v>
       </c>
       <c r="H13">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1408,7 +1958,7 @@
         <v>816</v>
       </c>
       <c r="M13">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N13">
         <v>4</v>
@@ -1420,7 +1970,7 @@
         <v>1344</v>
       </c>
       <c r="R13">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S13">
         <v>4</v>
@@ -1432,7 +1982,7 @@
         <v>1856</v>
       </c>
       <c r="AB13">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC13">
         <v>4</v>
@@ -1444,13 +1994,70 @@
         <v>2448</v>
       </c>
       <c r="AG13">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK13">
+        <v>6</v>
+      </c>
+      <c r="AL13">
+        <v>2176</v>
+      </c>
+      <c r="AM13">
+        <v>272</v>
+      </c>
+      <c r="AN13">
+        <v>16</v>
+      </c>
+      <c r="AO13">
+        <v>16</v>
+      </c>
+      <c r="AP13">
+        <v>3</v>
+      </c>
+      <c r="AQ13">
+        <v>9</v>
+      </c>
+      <c r="AR13">
+        <v>61001</v>
+      </c>
+      <c r="AS13">
+        <v>62001</v>
+      </c>
+      <c r="AT13">
+        <v>63001</v>
+      </c>
+      <c r="AU13">
+        <v>64001</v>
+      </c>
+      <c r="AV13">
+        <v>65001</v>
+      </c>
+      <c r="AW13">
+        <v>66001</v>
+      </c>
+      <c r="AX13">
+        <v>67001</v>
+      </c>
+      <c r="AY13">
+        <v>68001</v>
+      </c>
+      <c r="AZ13">
+        <v>69001</v>
+      </c>
+      <c r="BA13">
+        <v>60051</v>
+      </c>
+      <c r="BB13">
+        <v>60052</v>
+      </c>
+      <c r="BC13">
+        <v>60052</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1458,7 +2065,7 @@
         <v>208</v>
       </c>
       <c r="C14">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1470,7 +2077,7 @@
         <v>832</v>
       </c>
       <c r="H14">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1482,7 +2089,7 @@
         <v>832</v>
       </c>
       <c r="M14">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N14">
         <v>4</v>
@@ -1494,7 +2101,7 @@
         <v>1360</v>
       </c>
       <c r="R14">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S14">
         <v>4</v>
@@ -1506,7 +2113,7 @@
         <v>1872</v>
       </c>
       <c r="AB14">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC14">
         <v>4</v>
@@ -1518,13 +2125,70 @@
         <v>2464</v>
       </c>
       <c r="AG14">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AK14">
+        <v>6</v>
+      </c>
+      <c r="AL14">
+        <v>2144</v>
+      </c>
+      <c r="AM14">
+        <v>368</v>
+      </c>
+      <c r="AN14">
+        <v>16</v>
+      </c>
+      <c r="AO14">
+        <v>16</v>
+      </c>
+      <c r="AP14">
+        <v>3</v>
+      </c>
+      <c r="AQ14">
+        <v>3</v>
+      </c>
+      <c r="AR14">
+        <v>61000</v>
+      </c>
+      <c r="AS14">
+        <v>62000</v>
+      </c>
+      <c r="AT14">
+        <v>63000</v>
+      </c>
+      <c r="AU14">
+        <v>64000</v>
+      </c>
+      <c r="AV14">
+        <v>65000</v>
+      </c>
+      <c r="AW14">
+        <v>66000</v>
+      </c>
+      <c r="AX14">
+        <v>67000</v>
+      </c>
+      <c r="AY14">
+        <v>68000</v>
+      </c>
+      <c r="AZ14">
+        <v>69000</v>
+      </c>
+      <c r="BA14">
+        <v>60011</v>
+      </c>
+      <c r="BB14">
+        <v>60012</v>
+      </c>
+      <c r="BC14">
+        <v>60013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1532,7 +2196,7 @@
         <v>224</v>
       </c>
       <c r="C15">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -1544,7 +2208,7 @@
         <v>848</v>
       </c>
       <c r="H15">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1556,7 +2220,7 @@
         <v>848</v>
       </c>
       <c r="M15">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N15">
         <v>4</v>
@@ -1568,7 +2232,7 @@
         <v>1376</v>
       </c>
       <c r="R15">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S15">
         <v>4</v>
@@ -1580,7 +2244,7 @@
         <v>1888</v>
       </c>
       <c r="AB15">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC15">
         <v>4</v>
@@ -1592,13 +2256,13 @@
         <v>2480</v>
       </c>
       <c r="AG15">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1606,7 +2270,7 @@
         <v>240</v>
       </c>
       <c r="C16">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -1618,7 +2282,7 @@
         <v>864</v>
       </c>
       <c r="H16">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1630,7 +2294,7 @@
         <v>864</v>
       </c>
       <c r="M16">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N16">
         <v>4</v>
@@ -1642,7 +2306,7 @@
         <v>1392</v>
       </c>
       <c r="R16">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S16">
         <v>4</v>
@@ -1654,7 +2318,7 @@
         <v>1904</v>
       </c>
       <c r="AB16">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC16">
         <v>4</v>
@@ -1666,7 +2330,7 @@
         <v>2496</v>
       </c>
       <c r="AG16">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH16">
         <v>4</v>
@@ -1680,7 +2344,7 @@
         <v>256</v>
       </c>
       <c r="C17">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -1692,7 +2356,7 @@
         <v>880</v>
       </c>
       <c r="H17">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1704,7 +2368,7 @@
         <v>880</v>
       </c>
       <c r="M17">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N17">
         <v>4</v>
@@ -1716,7 +2380,7 @@
         <v>1408</v>
       </c>
       <c r="R17">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S17">
         <v>4</v>
@@ -1728,7 +2392,7 @@
         <v>1920</v>
       </c>
       <c r="AB17">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC17">
         <v>4</v>
@@ -1740,7 +2404,7 @@
         <v>2512</v>
       </c>
       <c r="AG17">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH17">
         <v>4</v>
@@ -1754,7 +2418,7 @@
         <v>272</v>
       </c>
       <c r="C18">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1766,7 +2430,7 @@
         <v>896</v>
       </c>
       <c r="H18">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -1778,7 +2442,7 @@
         <v>896</v>
       </c>
       <c r="M18">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N18">
         <v>4</v>
@@ -1790,7 +2454,7 @@
         <v>1424</v>
       </c>
       <c r="R18">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S18">
         <v>4</v>
@@ -1802,7 +2466,7 @@
         <v>1936</v>
       </c>
       <c r="AB18">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC18">
         <v>4</v>
@@ -1814,7 +2478,7 @@
         <v>2528</v>
       </c>
       <c r="AG18">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH18">
         <v>4</v>
@@ -1828,7 +2492,7 @@
         <v>288</v>
       </c>
       <c r="C19">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1840,7 +2504,7 @@
         <v>912</v>
       </c>
       <c r="H19">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1852,7 +2516,7 @@
         <v>912</v>
       </c>
       <c r="M19">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N19">
         <v>4</v>
@@ -1864,7 +2528,7 @@
         <v>1440</v>
       </c>
       <c r="R19">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S19">
         <v>4</v>
@@ -1876,7 +2540,7 @@
         <v>1952</v>
       </c>
       <c r="AB19">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC19">
         <v>4</v>
@@ -1888,7 +2552,7 @@
         <v>2544</v>
       </c>
       <c r="AG19">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH19">
         <v>4</v>
@@ -1902,7 +2566,7 @@
         <v>304</v>
       </c>
       <c r="C20">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1914,7 +2578,7 @@
         <v>928</v>
       </c>
       <c r="H20">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -1926,7 +2590,7 @@
         <v>928</v>
       </c>
       <c r="M20">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N20">
         <v>4</v>
@@ -1938,7 +2602,7 @@
         <v>1456</v>
       </c>
       <c r="R20">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S20">
         <v>4</v>
@@ -1950,7 +2614,7 @@
         <v>1968</v>
       </c>
       <c r="AB20">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC20">
         <v>4</v>
@@ -1962,7 +2626,7 @@
         <v>2560</v>
       </c>
       <c r="AG20">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH20">
         <v>4</v>
@@ -1976,7 +2640,7 @@
         <v>320</v>
       </c>
       <c r="C21">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -1988,7 +2652,7 @@
         <v>944</v>
       </c>
       <c r="H21">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -2000,7 +2664,7 @@
         <v>944</v>
       </c>
       <c r="M21">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N21">
         <v>4</v>
@@ -2012,7 +2676,7 @@
         <v>1472</v>
       </c>
       <c r="R21">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S21">
         <v>4</v>
@@ -2024,7 +2688,7 @@
         <v>1984</v>
       </c>
       <c r="AB21">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC21">
         <v>4</v>
@@ -2036,7 +2700,7 @@
         <v>2576</v>
       </c>
       <c r="AG21">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH21">
         <v>4</v>
@@ -2050,7 +2714,7 @@
         <v>336</v>
       </c>
       <c r="C22">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -2062,7 +2726,7 @@
         <v>960</v>
       </c>
       <c r="H22">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -2074,7 +2738,7 @@
         <v>960</v>
       </c>
       <c r="M22">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N22">
         <v>4</v>
@@ -2086,7 +2750,7 @@
         <v>1488</v>
       </c>
       <c r="R22">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="S22">
         <v>5</v>
@@ -2098,7 +2762,7 @@
         <v>2000</v>
       </c>
       <c r="AB22">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC22">
         <v>4</v>
@@ -2110,7 +2774,7 @@
         <v>2592</v>
       </c>
       <c r="AG22">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH22">
         <v>4</v>
@@ -2124,7 +2788,7 @@
         <v>352</v>
       </c>
       <c r="C23">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -2136,7 +2800,7 @@
         <v>976</v>
       </c>
       <c r="H23">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -2148,7 +2812,7 @@
         <v>976</v>
       </c>
       <c r="M23">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N23">
         <v>4</v>
@@ -2160,7 +2824,7 @@
         <v>2016</v>
       </c>
       <c r="AB23">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC23">
         <v>4</v>
@@ -2172,7 +2836,7 @@
         <v>2608</v>
       </c>
       <c r="AG23">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH23">
         <v>4</v>
@@ -2186,7 +2850,7 @@
         <v>368</v>
       </c>
       <c r="C24">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -2198,7 +2862,7 @@
         <v>992</v>
       </c>
       <c r="H24">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -2210,7 +2874,7 @@
         <v>992</v>
       </c>
       <c r="M24">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N24">
         <v>4</v>
@@ -2222,7 +2886,7 @@
         <v>2032</v>
       </c>
       <c r="AB24">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC24">
         <v>4</v>
@@ -2234,7 +2898,7 @@
         <v>2624</v>
       </c>
       <c r="AG24">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH24">
         <v>4</v>
@@ -2248,7 +2912,7 @@
         <v>384</v>
       </c>
       <c r="C25">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -2260,7 +2924,7 @@
         <v>1008</v>
       </c>
       <c r="H25">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -2272,7 +2936,7 @@
         <v>1008</v>
       </c>
       <c r="M25">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N25">
         <v>4</v>
@@ -2284,7 +2948,7 @@
         <v>2048</v>
       </c>
       <c r="AB25">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC25">
         <v>4</v>
@@ -2296,7 +2960,7 @@
         <v>2640</v>
       </c>
       <c r="AG25">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH25">
         <v>4</v>
@@ -2310,7 +2974,7 @@
         <v>400</v>
       </c>
       <c r="C26">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -2322,7 +2986,7 @@
         <v>1024</v>
       </c>
       <c r="H26">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -2334,7 +2998,7 @@
         <v>1024</v>
       </c>
       <c r="M26">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N26">
         <v>4</v>
@@ -2346,7 +3010,7 @@
         <v>2064</v>
       </c>
       <c r="AB26">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC26">
         <v>4</v>
@@ -2358,7 +3022,7 @@
         <v>2656</v>
       </c>
       <c r="AG26">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH26">
         <v>4</v>
@@ -2372,7 +3036,7 @@
         <v>416</v>
       </c>
       <c r="C27">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -2384,7 +3048,7 @@
         <v>1040</v>
       </c>
       <c r="H27">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -2396,7 +3060,7 @@
         <v>1040</v>
       </c>
       <c r="M27">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N27">
         <v>4</v>
@@ -2408,7 +3072,7 @@
         <v>2080</v>
       </c>
       <c r="AB27">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC27">
         <v>4</v>
@@ -2420,7 +3084,7 @@
         <v>2672</v>
       </c>
       <c r="AG27">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH27">
         <v>4</v>
@@ -2434,7 +3098,7 @@
         <v>432</v>
       </c>
       <c r="C28">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -2446,7 +3110,7 @@
         <v>1056</v>
       </c>
       <c r="H28">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -2458,7 +3122,7 @@
         <v>1056</v>
       </c>
       <c r="M28">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N28">
         <v>4</v>
@@ -2470,7 +3134,7 @@
         <v>2096</v>
       </c>
       <c r="AB28">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC28">
         <v>4</v>
@@ -2482,7 +3146,7 @@
         <v>2688</v>
       </c>
       <c r="AG28">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH28">
         <v>4</v>
@@ -2496,7 +3160,7 @@
         <v>448</v>
       </c>
       <c r="C29">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -2508,7 +3172,7 @@
         <v>1072</v>
       </c>
       <c r="H29">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="I29">
         <v>2</v>
@@ -2520,7 +3184,7 @@
         <v>1072</v>
       </c>
       <c r="M29">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="N29">
         <v>5</v>
@@ -2532,7 +3196,7 @@
         <v>2112</v>
       </c>
       <c r="AB29">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC29">
         <v>4</v>
@@ -2544,7 +3208,7 @@
         <v>2704</v>
       </c>
       <c r="AG29">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH29">
         <v>4</v>
@@ -2558,7 +3222,7 @@
         <v>464</v>
       </c>
       <c r="C30">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -2570,7 +3234,7 @@
         <v>2128</v>
       </c>
       <c r="AB30">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC30">
         <v>4</v>
@@ -2582,7 +3246,7 @@
         <v>2720</v>
       </c>
       <c r="AG30">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH30">
         <v>4</v>
@@ -2596,7 +3260,7 @@
         <v>480</v>
       </c>
       <c r="C31">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -2608,7 +3272,7 @@
         <v>2144</v>
       </c>
       <c r="AB31">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC31">
         <v>4</v>
@@ -2620,7 +3284,7 @@
         <v>2736</v>
       </c>
       <c r="AG31">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH31">
         <v>4</v>
@@ -2634,7 +3298,7 @@
         <v>496</v>
       </c>
       <c r="C32">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D32">
         <v>4</v>
@@ -2646,7 +3310,7 @@
         <v>2160</v>
       </c>
       <c r="AB32">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC32">
         <v>4</v>
@@ -2658,7 +3322,7 @@
         <v>2752</v>
       </c>
       <c r="AG32">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH32">
         <v>4</v>
@@ -2672,7 +3336,7 @@
         <v>512</v>
       </c>
       <c r="C33">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -2684,7 +3348,7 @@
         <v>2176</v>
       </c>
       <c r="AB33">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC33">
         <v>4</v>
@@ -2696,7 +3360,7 @@
         <v>2768</v>
       </c>
       <c r="AG33">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH33">
         <v>4</v>
@@ -2710,7 +3374,7 @@
         <v>528</v>
       </c>
       <c r="C34">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -2722,7 +3386,7 @@
         <v>2192</v>
       </c>
       <c r="AB34">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC34">
         <v>4</v>
@@ -2734,7 +3398,7 @@
         <v>2784</v>
       </c>
       <c r="AG34">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH34">
         <v>4</v>
@@ -2748,7 +3412,7 @@
         <v>544</v>
       </c>
       <c r="C35">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D35">
         <v>4</v>
@@ -2760,7 +3424,7 @@
         <v>2208</v>
       </c>
       <c r="AB35">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC35">
         <v>4</v>
@@ -2772,7 +3436,7 @@
         <v>2800</v>
       </c>
       <c r="AG35">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AH35">
         <v>5</v>
@@ -2786,7 +3450,7 @@
         <v>560</v>
       </c>
       <c r="C36">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -2798,7 +3462,7 @@
         <v>2224</v>
       </c>
       <c r="AB36">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="AC36">
         <v>5</v>
@@ -2812,7 +3476,7 @@
         <v>576</v>
       </c>
       <c r="C37">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D37">
         <v>4</v>
@@ -2826,7 +3490,7 @@
         <v>592</v>
       </c>
       <c r="C38">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D38">
         <v>4</v>
@@ -2840,7 +3504,7 @@
         <v>608</v>
       </c>
       <c r="C39">
-        <v>196</v>
+        <v>416</v>
       </c>
       <c r="D39">
         <v>5</v>

</xml_diff>